<commit_message>
Made changes to handle new line in linked issues
</commit_message>
<xml_diff>
--- a/Jira/JiraUpload.xlsx
+++ b/Jira/JiraUpload.xlsx
@@ -405,7 +405,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -461,40 +461,38 @@
     <t>Components</t>
   </si>
   <si>
+    <t>To verify that error warning appears if the user attempts to navigate outside of the stepper to another area of the product</t>
+  </si>
+  <si>
     <t>API</t>
   </si>
   <si>
+    <t>Quality Assurance</t>
+  </si>
+  <si>
+    <t>harshili.desai</t>
+  </si>
+  <si>
+    <t>Mediware123</t>
+  </si>
+  <si>
     <t>QA</t>
   </si>
   <si>
-    <t>Quality Assurance</t>
+    <t>team:echo</t>
   </si>
   <si>
     <t>Functional</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>team:echo</t>
-  </si>
-  <si>
-    <t>harshili.desai</t>
-  </si>
-  <si>
-    <t>MCTS-1484,MCTS-1483,MCTS-1443</t>
-  </si>
-  <si>
-    <t>Mediware123</t>
-  </si>
-  <si>
-    <t>To verify the functionality of BACK Button</t>
+    <t xml:space="preserve">MCTS-1443,MCTS-1484,MCTS-1483
+</t>
   </si>
   <si>
     <t>TRUE</t>
   </si>
   <si>
-    <t>QA-3301</t>
+    <t>QA-3323</t>
   </si>
 </sst>
 </file>
@@ -502,7 +500,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,28 +550,6 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -670,34 +646,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="2" fontId="2" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="4" fontId="2" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="4" fontId="2" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+  <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1003,7 +981,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,15 +1011,15 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>26</v>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1049,7 +1027,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1035,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1072,76 +1050,76 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultRowHeight="51.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="18.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="7" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="7" width="20.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="7" width="55.42578125" collapsed="true"/>
-    <col min="5" max="10" customWidth="true" style="7" width="19.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="7" width="18.42578125" collapsed="true"/>
-    <col min="12" max="16384" style="7" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="20.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="55.42578125" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" style="3" width="19.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="18.42578125" collapsed="true"/>
+    <col min="12" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="51.75" r="1" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row ht="15" r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="51.75" r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>25</v>
+      <c r="J2" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>